<commit_message>
adding sms mechanism, moving auth to config
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">SMG Cape Town Service Work Flow </t>
   </si>
@@ -83,16 +83,7 @@
     <t>08:00</t>
   </si>
   <si>
-    <t>08:15</t>
-  </si>
-  <si>
     <t>Jacqui</t>
-  </si>
-  <si>
-    <t>08:30</t>
-  </si>
-  <si>
-    <t>Walied</t>
   </si>
 </sst>
 </file>
@@ -403,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -433,10 +424,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -450,6 +437,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -465,7 +453,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,24 +750,24 @@
     <col min="7" max="8" width="9.140625" style="18"/>
     <col min="9" max="9" width="17.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="39" customWidth="1"/>
+    <col min="11" max="11" width="17" style="37" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="41"/>
       <c r="K1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
@@ -790,15 +777,15 @@
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="8"/>
       <c r="L2" s="2"/>
       <c r="M2" s="3"/>
@@ -869,225 +856,135 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="17">
-        <v>27715359443</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="38">
+        <v>27626969018</v>
       </c>
       <c r="E5" s="16"/>
       <c r="I5" s="19"/>
       <c r="K5" s="20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
-        <v>3</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="17">
-        <v>27715359443</v>
-      </c>
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="16"/>
-      <c r="I6" s="19"/>
-      <c r="K6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="J6" s="24"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
-        <v>4</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="17">
-        <v>27715359443</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="I7" s="19"/>
-      <c r="K7" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="45">
-        <v>27626969018</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="I8" s="19"/>
-      <c r="K8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
-        <v>6</v>
-      </c>
+      <c r="A9" s="22"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="45">
-        <v>27626969018</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
-        <v>7</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="45">
-        <v>27626969018</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="25"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
-        <v>8</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="45">
-        <v>27626969018</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="J11" s="26"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="20"/>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="25"/>
-      <c r="J12" s="24"/>
+      <c r="B12" s="25"/>
       <c r="K12" s="20"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="J13" s="24"/>
+      <c r="B13" s="25"/>
       <c r="K13" s="20"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
+      <c r="B14" s="29"/>
       <c r="K14" s="20"/>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
       <c r="K15" s="20"/>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="30"/>
       <c r="K16" s="20"/>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
       <c r="K17" s="20"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34"/>
       <c r="K18" s="20"/>
       <c r="L18" s="2"/>
     </row>
@@ -1213,113 +1110,78 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="K43" s="20"/>
+      <c r="K43" s="8"/>
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="2"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="27"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="2"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="27"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="2"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="27"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="2"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="27"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
-      <c r="K48" s="20"/>
-      <c r="L48" s="2"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="27"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="22"/>
-      <c r="K49" s="20"/>
-      <c r="L49" s="2"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="27"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
       <c r="K50" s="8"/>
-      <c r="L50" s="2"/>
+      <c r="L50" s="27"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
       <c r="K51" s="8"/>
-      <c r="L51" s="29"/>
+      <c r="L51" s="33"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="22"/>
       <c r="K52" s="8"/>
-      <c r="L52" s="29"/>
+      <c r="L52" s="27"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="22"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="29"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="35"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="22"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="29"/>
+      <c r="K54" s="34"/>
+      <c r="L54" s="35"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="29"/>
+      <c r="K55" s="34"/>
+      <c r="L55" s="35"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="22"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="29"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K56" s="34"/>
+      <c r="L56" s="35"/>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="22"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="29"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="35"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="29"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="K60" s="36"/>
-      <c r="L60" s="37"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="K61" s="36"/>
-      <c r="L61" s="37"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="K62" s="36"/>
-      <c r="L62" s="37"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="K63" s="36"/>
-      <c r="L63" s="37"/>
-    </row>
-    <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="22"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="37"/>
+      <c r="K57" s="36"/>
+      <c r="L57" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>